<commit_message>
I added an icon
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -456,11 +456,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="A1" t="inlineStr"/>
       <c r="B1" t="inlineStr">
         <is>
           <t>False</t>
@@ -468,11 +464,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
           <t>False</t>
@@ -480,11 +472,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
           <t>False</t>
@@ -492,11 +480,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
           <t>False</t>
@@ -504,11 +488,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
           <t>False</t>

</xml_diff>

<commit_message>
I added a dropdown to switch to different days and I created a function that saves each task for each different day
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1930" yWindow="70" windowWidth="15200" windowHeight="8400" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -444,10 +444,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -458,12 +458,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Read Chapters 21-23</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
           <t>False</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Read Chapters 24-25</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Read Chapters 26-29</t>
         </is>
       </c>
     </row>
@@ -478,6 +488,11 @@
           <t>False</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -490,6 +505,11 @@
           <t>False</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -502,6 +522,11 @@
           <t>False</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -512,6 +537,11 @@
       <c r="B5" t="inlineStr">
         <is>
           <t>False</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
I fixed some mistakes I made
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -456,62 +456,146 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Coding</t>
-        </is>
-      </c>
+      <c r="A1" t="inlineStr"/>
       <c r="B1" t="inlineStr">
         <is>
           <t>False</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Robotics</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
           <t>False</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Princeton Review</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
           <t>False</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Violin</t>
+          <t>Read Chapters 1-3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>False</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Read Chapters 4-6 </t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Read Chapters 7-8</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Read Chapters 9-10</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Read Chapters 11-13</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Read Bowditch</t>
-        </is>
-      </c>
+      <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
           <t>False</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
I created the code to save the data for each textbox on each day.
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1930" yWindow="70" windowWidth="15200" windowHeight="8400" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -444,75 +444,171 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
     <col width="19.54296875" customWidth="1" min="1" max="1"/>
+    <col width="16.1796875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="16.1796875" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="17.26953125" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="18.26953125" bestFit="1" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr"/>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t> </t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t> </t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t> </t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>False</t>
@@ -520,29 +616,69 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t> </t>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t> </t>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t> </t>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Read Chapters 1-3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -552,27 +688,71 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Read Chapters 4-6 </t>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Read Chapters 7-8</t>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Read Chapters 9-10</t>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Read Chapters 11-13</t>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>False</t>
@@ -580,22 +760,62 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t> </t>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t> </t>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> 5</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t> </t>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
     </row>

</xml_diff>